<commit_message>
Added some data for datasets and a bit of analysis
</commit_message>
<xml_diff>
--- a/Data/CR_by_child_tsi.xlsx
+++ b/Data/CR_by_child_tsi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\UNISI\ENS Traineeship\GIT\LangComplexity\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57AA13D2-5665-4352-AC20-1F62DEA0F75D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C761320-0803-4299-8DA8-968CC5AE8642}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CR_by_child_tsi" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t>corpus</t>
   </si>
   <si>
-    <t>Syllable.complexity</t>
-  </si>
-  <si>
     <t>C_count</t>
   </si>
   <si>
@@ -251,12 +248,15 @@
   </si>
   <si>
     <t>5DB0A3B8000332FR_653</t>
+  </si>
+  <si>
+    <t>Syllable complexity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1090,10 +1090,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1117,16 +1119,16 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1134,25 +1136,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>0.35820895522388102</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>32.533333333333303</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>25</v>
@@ -1161,7 +1163,7 @@
         <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1169,25 +1171,25 @@
         <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>0.219512195121951</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>31.733333333333299</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3">
         <v>25</v>
@@ -1196,7 +1198,7 @@
         <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1204,25 +1206,25 @@
         <v>306</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>0.544303797468354</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>36.533333333333303</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4">
         <v>25</v>
@@ -1231,7 +1233,7 @@
         <v>18</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1239,25 +1241,25 @@
         <v>437</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>0.44736842105263203</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>39.066666666666698</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5">
         <v>25</v>
@@ -1266,7 +1268,7 @@
         <v>18</v>
       </c>
       <c r="K5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1274,25 +1276,25 @@
         <v>548</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>0.391891891891892</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>54.7</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6">
         <v>25</v>
@@ -1301,7 +1303,7 @@
         <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1309,25 +1311,25 @@
         <v>683</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>0.52631578947368396</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>59.7</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7">
         <v>25</v>
@@ -1336,7 +1338,7 @@
         <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1344,25 +1346,25 @@
         <v>819</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>0.469879518072289</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>24.366666666666699</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I8">
         <v>25</v>
@@ -1371,7 +1373,7 @@
         <v>18</v>
       </c>
       <c r="K8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1379,25 +1381,25 @@
         <v>967</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>0.26</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>30.566666666666698</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9">
         <v>25</v>
@@ -1406,7 +1408,7 @@
         <v>18</v>
       </c>
       <c r="K9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1414,25 +1416,25 @@
         <v>1131</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>0.18867924528301899</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <v>19.733333333333299</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I10">
         <v>25</v>
@@ -1441,7 +1443,7 @@
         <v>18</v>
       </c>
       <c r="K10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1449,25 +1451,25 @@
         <v>1271</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>0.439024390243902</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11">
         <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I11">
         <v>25</v>
@@ -1476,7 +1478,7 @@
         <v>18</v>
       </c>
       <c r="K11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1484,25 +1486,25 @@
         <v>1401</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>0.49504950495049499</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12">
         <v>51.9</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I12">
         <v>25</v>
@@ -1511,7 +1513,7 @@
         <v>18</v>
       </c>
       <c r="K12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1519,25 +1521,25 @@
         <v>1540</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13">
         <v>0.30769230769230799</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13">
         <v>8.1999999999999993</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I13">
         <v>25</v>
@@ -1546,7 +1548,7 @@
         <v>18</v>
       </c>
       <c r="K13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1554,25 +1556,25 @@
         <v>1665</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14">
         <v>0.35483870967741898</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14">
         <v>15.466666666666701</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I14">
         <v>25</v>
@@ -1581,7 +1583,7 @@
         <v>18</v>
       </c>
       <c r="K14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1589,25 +1591,25 @@
         <v>1802</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15">
         <v>0.42028985507246402</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15">
         <v>33.033333333333303</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I15">
         <v>25</v>
@@ -1616,7 +1618,7 @@
         <v>18</v>
       </c>
       <c r="K15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1624,25 +1626,25 @@
         <v>1920</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>0.44444444444444398</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16">
         <v>30.8333333333333</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I16">
         <v>25</v>
@@ -1651,7 +1653,7 @@
         <v>18</v>
       </c>
       <c r="K16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1659,25 +1661,25 @@
         <v>2047</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17">
         <v>0.46067415730337102</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17">
         <v>54.966666666666697</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I17">
         <v>25</v>
@@ -1686,7 +1688,7 @@
         <v>18</v>
       </c>
       <c r="K17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1694,25 +1696,25 @@
         <v>2182</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18">
         <v>0.30666666666666698</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18">
         <v>24.633333333333301</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I18">
         <v>25</v>
@@ -1721,7 +1723,7 @@
         <v>18</v>
       </c>
       <c r="K18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1729,25 +1731,25 @@
         <v>2324</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19">
         <v>0.53030303030303005</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19">
         <v>49.1</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I19">
         <v>25</v>
@@ -1756,7 +1758,7 @@
         <v>18</v>
       </c>
       <c r="K19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1764,25 +1766,25 @@
         <v>2479</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20">
         <v>0.28070175438596501</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20">
         <v>20.033333333333299</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I20">
         <v>25</v>
@@ -1791,7 +1793,7 @@
         <v>18</v>
       </c>
       <c r="K20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1799,25 +1801,25 @@
         <v>2608</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21">
         <v>0.43333333333333302</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21">
         <v>49.266666666666701</v>
       </c>
       <c r="F21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I21">
         <v>25</v>
@@ -1826,7 +1828,7 @@
         <v>18</v>
       </c>
       <c r="K21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1834,25 +1836,25 @@
         <v>2718</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22">
         <v>0.683168316831683</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22">
         <v>60.466666666666697</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I22">
         <v>25</v>
@@ -1861,7 +1863,7 @@
         <v>18</v>
       </c>
       <c r="K22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1869,25 +1871,25 @@
         <v>2855</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23">
         <v>0.5625</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23">
         <v>71.933333333333294</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I23">
         <v>25</v>
@@ -1896,7 +1898,7 @@
         <v>18</v>
       </c>
       <c r="K23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1904,25 +1906,25 @@
         <v>2974</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24">
         <v>0.58333333333333304</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24">
         <v>60.5</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I24">
         <v>25</v>
@@ -1931,7 +1933,7 @@
         <v>18</v>
       </c>
       <c r="K24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1939,25 +1941,25 @@
         <v>3132</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25">
         <v>0.261538461538462</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E25">
         <v>15.4333333333333</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I25">
         <v>25</v>
@@ -1966,7 +1968,7 @@
         <v>18</v>
       </c>
       <c r="K25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1974,25 +1976,25 @@
         <v>3253</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26">
         <v>0.34090909090909099</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26">
         <v>44.5</v>
       </c>
       <c r="F26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I26">
         <v>25</v>
@@ -2001,7 +2003,7 @@
         <v>18</v>
       </c>
       <c r="K26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2009,25 +2011,25 @@
         <v>3353</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27">
         <v>0.58064516129032295</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E27">
         <v>67.3333333333333</v>
       </c>
       <c r="F27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I27">
         <v>25</v>
@@ -2036,7 +2038,7 @@
         <v>18</v>
       </c>
       <c r="K27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2044,25 +2046,25 @@
         <v>3468</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28">
         <v>0.22077922077922099</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E28">
         <v>18.3333333333333</v>
       </c>
       <c r="F28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I28">
         <v>25</v>
@@ -2071,7 +2073,7 @@
         <v>18</v>
       </c>
       <c r="K28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2079,25 +2081,25 @@
         <v>3603</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29">
         <v>0.62385321100917401</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E29">
         <v>63.266666666666701</v>
       </c>
       <c r="F29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I29">
         <v>25</v>
@@ -2106,7 +2108,7 @@
         <v>18</v>
       </c>
       <c r="K29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2114,25 +2116,25 @@
         <v>3735</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30">
         <v>0.65972222222222199</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E30">
         <v>68.3333333333333</v>
       </c>
       <c r="F30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I30">
         <v>25</v>
@@ -2141,7 +2143,7 @@
         <v>18</v>
       </c>
       <c r="K30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2149,25 +2151,25 @@
         <v>3906</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31">
         <v>0.35106382978723399</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E31">
         <v>41.8</v>
       </c>
       <c r="F31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I31">
         <v>25</v>
@@ -2176,7 +2178,7 @@
         <v>18</v>
       </c>
       <c r="K31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -2184,25 +2186,25 @@
         <v>4049</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32">
         <v>0.46808510638297901</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E32">
         <v>28.3333333333333</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I32">
         <v>25</v>
@@ -2211,7 +2213,7 @@
         <v>18</v>
       </c>
       <c r="K32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2219,25 +2221,25 @@
         <v>4205</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C33">
         <v>0.480769230769231</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E33">
         <v>21.766666666666701</v>
       </c>
       <c r="F33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I33">
         <v>25</v>
@@ -2246,7 +2248,7 @@
         <v>18</v>
       </c>
       <c r="K33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>